<commit_message>
using course code spreadsheet for organisation detection as well
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -671,7 +671,7 @@
     </row>
     <row r="8" xml:space="preserve">
       <c r="A8" t="str">
-        <v>Lääketieteellinen: psykologia, soveltava psykologia ja logopedia</v>
+        <v>H30</v>
       </c>
       <c r="B8" t="str" xml:space="preserve">
         <v xml:space="preserve">KK-ENERI_x000d_
@@ -681,39 +681,55 @@
 KK-ENG301_x000d_
 KK-ENG302_x000d_
 KK-ENG303</v>
-      </c>
-      <c r="C8" t="str">
-        <v xml:space="preserve">KK-AIAKVU2OP </v>
-      </c>
-      <c r="D8" t="str">
-        <v xml:space="preserve">KK-AIAKTE1OP </v>
-      </c>
-      <c r="E8" t="str">
-        <v xml:space="preserve">KK-MOAKKO2SP </v>
-      </c>
-      <c r="F8" t="str">
-        <v xml:space="preserve">KK-MOAKSK1SP </v>
-      </c>
-      <c r="G8" t="str" xml:space="preserve">
-        <v xml:space="preserve">KK-RULAAK_x000d_
-KK-RUKAIKKI_x000d_
-KK-RUERI_x000d_
-KK-RUO204_x000d_
-KK-RUO205_x000d_
-KK-RUO206</v>
-      </c>
-      <c r="H8" t="str" xml:space="preserve">
-        <v xml:space="preserve">KK-FINMU _x000d_
-KK-FIN01 _x000d_
-KK-FIN02 _x000d_
-KK-FIN08 </v>
       </c>
     </row>
     <row r="9" xml:space="preserve">
       <c r="A9" t="str">
+        <v>4141</v>
+      </c>
+      <c r="B9" t="str" xml:space="preserve">
+        <v xml:space="preserve">KK-ENERI_x000d_
+KK-ENKAIKKI_x000d_
+KK-ENKAIKKI1/2_x000d_
+KK-ENLAAK_x000d_
+KK-ENG301_x000d_
+KK-ENG302_x000d_
+KK-ENG303</v>
+      </c>
+    </row>
+    <row r="10" xml:space="preserve">
+      <c r="A10" t="str">
+        <v>414</v>
+      </c>
+      <c r="B10" t="str" xml:space="preserve">
+        <v xml:space="preserve">KK-ENERI_x000d_
+KK-ENKAIKKI_x000d_
+KK-ENKAIKKI1/2_x000d_
+KK-ENLAAK_x000d_
+KK-ENG301_x000d_
+KK-ENG302_x000d_
+KK-ENG303</v>
+      </c>
+    </row>
+    <row r="11" xml:space="preserve">
+      <c r="A11" t="str">
+        <v>H3456</v>
+      </c>
+      <c r="B11" t="str" xml:space="preserve">
+        <v xml:space="preserve">KK-ENERI_x000d_
+KK-ENKAIKKI_x000d_
+KK-ENKAIKKI1/2_x000d_
+KK-ENLAAK_x000d_
+KK-ENG301_x000d_
+KK-ENG302_x000d_
+KK-ENG303</v>
+      </c>
+    </row>
+    <row r="12" xml:space="preserve">
+      <c r="A12" t="str">
         <v>H80</v>
       </c>
-      <c r="B9" t="str" xml:space="preserve">
+      <c r="B12" t="str" xml:space="preserve">
         <v xml:space="preserve">KK-ENERI_x000d_
 KK-ENKAIKKI_x000d_
 KK-ENKAIKKI1/2_x000d_
@@ -724,19 +740,19 @@
 KK-ENG302_x000d_
 KK-ENG303</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C12" t="str">
         <v xml:space="preserve">KK-AIAKVU1OP </v>
       </c>
-      <c r="D9" t="str">
+      <c r="D12" t="str">
         <v xml:space="preserve">KK-AIAKTE2OP </v>
       </c>
-      <c r="E9" t="str">
+      <c r="E12" t="str">
         <v xml:space="preserve">KK-MOAKKO1SP </v>
       </c>
-      <c r="F9" t="str">
+      <c r="F12" t="str">
         <v xml:space="preserve">KK-MOAKSK2SP </v>
       </c>
-      <c r="G9" t="str" xml:space="preserve">
+      <c r="G12" t="str" xml:space="preserve">
         <v xml:space="preserve">KK-RUMAME_x000d_
 KK-RUKAIKKI_x000d_
 KK-RUERI_x000d_
@@ -744,18 +760,18 @@
 KK-RUO205_x000d_
 KK-RUO206</v>
       </c>
-      <c r="H9" t="str" xml:space="preserve">
+      <c r="H12" t="str" xml:space="preserve">
         <v xml:space="preserve">KK-FINMU _x000d_
 KK-FIN01 _x000d_
 KK-FIN02 _x000d_
 KK-FIN08 </v>
       </c>
     </row>
-    <row r="10" xml:space="preserve">
-      <c r="A10" t="str">
+    <row r="13" xml:space="preserve">
+      <c r="A13" t="str">
         <v>H50</v>
       </c>
-      <c r="B10" t="str" xml:space="preserve">
+      <c r="B13" t="str" xml:space="preserve">
         <v xml:space="preserve">KK-ENERI_x000d_
 KK-ENKAIKKI_x000d_
 KK-ENKAIKKI1/2_x000d_
@@ -766,19 +782,19 @@
 KK-ENG302_x000d_
 KK-ENG303</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C13" t="str">
         <v xml:space="preserve">KK-AIAKVU1OP </v>
       </c>
-      <c r="D10" t="str">
+      <c r="D13" t="str">
         <v xml:space="preserve">KK-AIAKTE2OP </v>
       </c>
-      <c r="E10" t="str">
+      <c r="E13" t="str">
         <v xml:space="preserve">KK-MOAKKO1SP </v>
       </c>
-      <c r="F10" t="str">
+      <c r="F13" t="str">
         <v xml:space="preserve">KK-MOAKSK2SP </v>
       </c>
-      <c r="G10" t="str" xml:space="preserve">
+      <c r="G13" t="str" xml:space="preserve">
         <v xml:space="preserve">KK-RUMALU_x000d_
 KK-RUKAIKKI_x000d_
 KK-RUERI_x000d_
@@ -786,18 +802,18 @@
 KK-RUO205_x000d_
 KK-RUO206</v>
       </c>
-      <c r="H10" t="str" xml:space="preserve">
+      <c r="H13" t="str" xml:space="preserve">
         <v xml:space="preserve">KK-FINMU _x000d_
 KK-FIN01 _x000d_
 KK-FIN02 _x000d_
 KK-FIN08 </v>
       </c>
     </row>
-    <row r="11" xml:space="preserve">
-      <c r="A11" t="str">
+    <row r="14" xml:space="preserve">
+      <c r="A14" t="str">
         <v>H20</v>
       </c>
-      <c r="B11" t="str" xml:space="preserve">
+      <c r="B14" t="str" xml:space="preserve">
         <v xml:space="preserve">KK-ENERI_x000d_
 KK-ENKAIKKI_x000d_
 KK-ENKAIKKI1/2_x000d_
@@ -806,19 +822,19 @@
 KK-ENG302_x000d_
 KK-ENG303</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C14" t="str">
         <v>KK-AIAKVU1OP</v>
       </c>
-      <c r="D11" t="str">
+      <c r="D14" t="str">
         <v xml:space="preserve">KK-AIAKTE2OP </v>
       </c>
-      <c r="E11" t="str">
+      <c r="E14" t="str">
         <v xml:space="preserve">KK-MOAKKO1SP </v>
       </c>
-      <c r="F11" t="str">
+      <c r="F14" t="str">
         <v xml:space="preserve">KK-MOAKSK2SP </v>
       </c>
-      <c r="G11" t="str" xml:space="preserve">
+      <c r="G14" t="str" xml:space="preserve">
         <v xml:space="preserve">KK-RUOIK_x000d_
 KK-RUKAIKKI_x000d_
 KK-RUERI_x000d_
@@ -826,18 +842,18 @@
 KK-RUO205_x000d_
 KK-RUO206</v>
       </c>
-      <c r="H11" t="str" xml:space="preserve">
+      <c r="H14" t="str" xml:space="preserve">
         <v xml:space="preserve">KK-FINMU _x000d_
 KK-FIN01 _x000d_
 KK-FIN02 _x000d_
 KK-FIN08 </v>
       </c>
     </row>
-    <row r="12" xml:space="preserve">
-      <c r="A12" t="str">
+    <row r="15" xml:space="preserve">
+      <c r="A15" t="str">
         <v>H74</v>
       </c>
-      <c r="B12" t="str" xml:space="preserve">
+      <c r="B15" t="str" xml:space="preserve">
         <v xml:space="preserve">KK-ENERI_x000d_
 KK-ENKAIKKI_x000d_
 KK-ENKAIKKI1/2_x000d_
@@ -846,19 +862,19 @@
 KK-ENG302_x000d_
 KK-ENG303</v>
       </c>
-      <c r="C12" t="str">
+      <c r="C15" t="str">
         <v xml:space="preserve">KK-AIAKVU1OP </v>
       </c>
-      <c r="D12" t="str">
+      <c r="D15" t="str">
         <v xml:space="preserve">KK-AIAKTE2OP </v>
       </c>
-      <c r="E12" t="str">
+      <c r="E15" t="str">
         <v xml:space="preserve">KK-MOAKKO1SP </v>
       </c>
-      <c r="F12" t="str">
+      <c r="F15" t="str">
         <v xml:space="preserve">KK-MOAKSK2SP </v>
       </c>
-      <c r="G12" t="str" xml:space="preserve">
+      <c r="G15" t="str" xml:space="preserve">
         <v xml:space="preserve">KK-RUVALT_x000d_
 KK-RUKAIKKI_x000d_
 KK-RUERI_x000d_
@@ -866,18 +882,18 @@
 KK-RUO205_x000d_
 KK-RUO206</v>
       </c>
-      <c r="H12" t="str" xml:space="preserve">
+      <c r="H15" t="str" xml:space="preserve">
         <v xml:space="preserve">KK-FINMU _x000d_
 KK-FIN01 _x000d_
 KK-FIN02 _x000d_
 KK-FIN08</v>
       </c>
     </row>
-    <row r="13" xml:space="preserve">
-      <c r="A13" t="str">
+    <row r="16" xml:space="preserve">
+      <c r="A16" t="str">
         <v>H10</v>
       </c>
-      <c r="B13" t="str" xml:space="preserve">
+      <c r="B16" t="str" xml:space="preserve">
         <v xml:space="preserve">KK-ENERI_x000d_
 KK-ENKAIKKI_x000d_
 KK-ENKAIKKI1/2_x000d_
@@ -886,19 +902,19 @@
 KK-ENG302_x000d_
 KK-ENG303</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C16" t="str">
         <v xml:space="preserve">KK-AIAKVU1OP  </v>
       </c>
-      <c r="D13" t="str">
+      <c r="D16" t="str">
         <v xml:space="preserve">KK-AIAKTE2OP </v>
       </c>
-      <c r="E13" t="str">
+      <c r="E16" t="str">
         <v xml:space="preserve">KK-MOAKKO1SP </v>
       </c>
-      <c r="F13" t="str">
+      <c r="F16" t="str">
         <v xml:space="preserve">KK-MOAKSK2SP </v>
       </c>
-      <c r="G13" t="str" xml:space="preserve">
+      <c r="G16" t="str" xml:space="preserve">
         <v xml:space="preserve">KK-RUTEOL_x000d_
 KK-RUKAIKKI_x000d_
 KK-RUERI_x000d_
@@ -906,18 +922,18 @@
 KK-RUO205_x000d_
 KK-RUO206</v>
       </c>
-      <c r="H13" t="str" xml:space="preserve">
+      <c r="H16" t="str" xml:space="preserve">
         <v xml:space="preserve">KK-FINMU _x000d_
 KK-FIN01 _x000d_
 KK-FIN02 _x000d_
 KK-FIN08</v>
       </c>
     </row>
-    <row r="14" xml:space="preserve">
-      <c r="A14" t="str">
+    <row r="17" xml:space="preserve">
+      <c r="A17" t="str">
         <v>H70</v>
       </c>
-      <c r="B14" t="str" xml:space="preserve">
+      <c r="B17" t="str" xml:space="preserve">
         <v xml:space="preserve">KK-ENERI_x000d_
 KK-ENKAIKKI_x000d_
 KK-ENKAIKKI1/2_x000d_
@@ -926,19 +942,19 @@
 KK-ENG302_x000d_
 KK-ENG303</v>
       </c>
-      <c r="C14" t="str">
+      <c r="C17" t="str">
         <v xml:space="preserve">KK-AIAKVU2OP </v>
       </c>
-      <c r="D14" t="str">
+      <c r="D17" t="str">
         <v xml:space="preserve">KK-AIAKTE2OP </v>
       </c>
-      <c r="E14" t="str">
+      <c r="E17" t="str">
         <v xml:space="preserve">KK-MOAKKO2SP </v>
       </c>
-      <c r="F14" t="str">
+      <c r="F17" t="str">
         <v xml:space="preserve">KK-MOAKSK2SP </v>
       </c>
-      <c r="G14" t="str" xml:space="preserve">
+      <c r="G17" t="str" xml:space="preserve">
         <v xml:space="preserve">KK-RUVALT_x000d_
 KK-RUKAIKKI_x000d_
 KK-RUERI_x000d_
@@ -946,7 +962,7 @@
 KK-RUO205_x000d_
 KK-RUO206</v>
       </c>
-      <c r="H14" t="str" xml:space="preserve">
+      <c r="H17" t="str" xml:space="preserve">
         <v xml:space="preserve">KK-FINMU _x000d_
 KK-FIN01 _x000d_
 KK-FIN02 _x000d_
@@ -955,7 +971,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H17"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>